<commit_message>
added 2kr of mean packets in buffer
</commit_message>
<xml_diff>
--- a/excel/FactorialAnalysis_Throughput.xlsx
+++ b/excel/FactorialAnalysis_Throughput.xlsx
@@ -1103,7 +1103,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1743,11 +1743,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="49706094"/>
-        <c:axId val="57780044"/>
+        <c:axId val="83871853"/>
+        <c:axId val="6037251"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49706094"/>
+        <c:axId val="83871853"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1789,12 +1789,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57780044"/>
+        <c:crossAx val="6037251"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57780044"/>
+        <c:axId val="6037251"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,7 +1836,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49706094"/>
+        <c:crossAx val="83871853"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1864,7 +1864,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2452,11 +2452,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="94577709"/>
-        <c:axId val="19787567"/>
+        <c:axId val="77081031"/>
+        <c:axId val="90626808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94577709"/>
+        <c:axId val="77081031"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2498,12 +2498,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19787567"/>
+        <c:crossAx val="90626808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="19787567"/>
+        <c:axId val="90626808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2545,7 +2545,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94577709"/>
+        <c:crossAx val="77081031"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2639,48 +2639,48 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{3477F28B-D343-47A1-865A-C71FCA758450}">
-  <header guid="{DB0DE62B-4E3E-47F1-9B4C-A28B42090C1C}" dateTime="2021-01-26T16:06:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="15" maxSheetId="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{95955010-3D96-4B27-BC2A-E42D6F5943AA}">
+  <header guid="{91FCEA43-B60C-4872-AC04-26CC4B261FF2}" dateTime="2021-01-26T16:06:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="15" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{6F5D2B03-D338-4567-9742-8341EEF4F638}" dateTime="2021-01-26T16:07:00.000000000Z" userName=" " r:id="rId2" minRId="16" maxRId="65" maxSheetId="2">
+  <header guid="{986E47CE-6530-4190-A8A7-8EEE371D9150}" dateTime="2021-01-26T16:07:00.000000000Z" userName=" " r:id="rId2" minRId="16" maxRId="65" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{43193C1C-1CD2-4C86-90F0-595DBA491B1B}" dateTime="2021-01-26T16:09:00.000000000Z" userName=" " r:id="rId3" minRId="66" maxRId="70" maxSheetId="2">
+  <header guid="{41310214-2A2C-49CC-983D-13F5271EAB39}" dateTime="2021-01-26T16:09:00.000000000Z" userName=" " r:id="rId3" minRId="66" maxRId="70" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{16A00CEC-9FF4-4009-B9B0-AD2E62F11FC3}" dateTime="2021-01-26T16:12:00.000000000Z" userName=" " r:id="rId4" minRId="71" maxRId="150" maxSheetId="2">
+  <header guid="{080B53E9-F857-45AB-8580-DF44DF4F025F}" dateTime="2021-01-26T16:12:00.000000000Z" userName=" " r:id="rId4" minRId="71" maxRId="150" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{3B19B3AA-3DD7-466C-9C77-762955EE110C}" dateTime="2021-01-26T16:13:00.000000000Z" userName=" " r:id="rId5" minRId="151" maxRId="310" maxSheetId="2">
+  <header guid="{D2DC5D1F-1880-473B-A065-0BD5A7C35098}" dateTime="2021-01-26T16:13:00.000000000Z" userName=" " r:id="rId5" minRId="151" maxRId="310" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{AA8A20A3-84B2-4BA8-A8BE-8BCB92E376D1}" dateTime="2021-01-26T16:16:00.000000000Z" userName=" " r:id="rId6" minRId="311" maxRId="315" maxSheetId="2">
+  <header guid="{63CC5E7B-CCE2-4908-AB23-3C57AE07DAE4}" dateTime="2021-01-26T16:16:00.000000000Z" userName=" " r:id="rId6" minRId="311" maxRId="315" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{BFA2E9E6-B55C-4EF8-8D27-0B7AC6F5CB11}" dateTime="2021-01-26T16:20:00.000000000Z" userName=" " r:id="rId7" minRId="316" maxRId="795" maxSheetId="2">
+  <header guid="{59502184-712E-4375-A5AA-7BC90E6AE507}" dateTime="2021-01-26T16:20:00.000000000Z" userName=" " r:id="rId7" minRId="316" maxRId="795" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{98453688-244F-48AA-8AEA-9C75EADFFF81}" dateTime="2021-01-26T16:21:00.000000000Z" userName=" " r:id="rId8" minRId="796" maxRId="880" maxSheetId="2">
+  <header guid="{F0990949-CC0F-47F3-BE83-53BF5060020C}" dateTime="2021-01-26T16:21:00.000000000Z" userName=" " r:id="rId8" minRId="796" maxRId="880" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{3477F28B-D343-47A1-865A-C71FCA758450}" dateTime="2021-01-26T16:22:00.000000000Z" userName=" " r:id="rId9" minRId="881" maxRId="883" maxSheetId="2">
+  <header guid="{95955010-3D96-4B27-BC2A-E42D6F5943AA}" dateTime="2021-01-26T16:22:00.000000000Z" userName=" " r:id="rId9" minRId="881" maxRId="883" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -7527,7 +7527,7 @@
   </sheetPr>
   <dimension ref="B1:AY225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H58" activeCellId="0" sqref="H58"/>
     </sheetView>
   </sheetViews>

</xml_diff>